<commit_message>
Fix flag to await backend return
</commit_message>
<xml_diff>
--- a/sources/ModeloNEOEdited.xlsx
+++ b/sources/ModeloNEOEdited.xlsx
@@ -3268,46 +3268,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>8</col>
-      <colOff>247650</colOff>
-      <row>0</row>
-      <rowOff>66675</rowOff>
-    </from>
-    <ext cx="1466850" cy="409575"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="image1.png"/>
-        <cNvPicPr preferRelativeResize="0"/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:xfrm>
-          <a:off x="13916025" y="66675"/>
-          <a:ext cx="1466850" cy="409575"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData fLocksWithSheet="0"/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -3375,45 +3335,10 @@
     </graphicFrame>
     <clientData fLocksWithSheet="0"/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>428625</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1562100" cy="400050"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="image2.png"/>
-        <cNvPicPr preferRelativeResize="0"/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:xfrm>
-          <a:off x="12011025" y="0"/>
-          <a:ext cx="1562100" cy="400050"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData fLocksWithSheet="0"/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
@@ -3442,42 +3367,6 @@
     </graphicFrame>
     <clientData/>
   </twoCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>1184276</colOff>
-      <row>0</row>
-      <rowOff>53940</rowOff>
-    </from>
-    <ext cx="1473140" cy="414055"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Imagem 2"/>
-        <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </cNvPicPr>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:xfrm>
-          <a:off x="10118726" y="53940"/>
-          <a:ext cx="1473140" cy="414055"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -8911,7 +8800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9880,7 +9769,6 @@
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" paperSize="9" scale="57"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31700,10 +31588,34 @@
       <c r="R3" t="n">
         <v>23399.91</v>
       </c>
-      <c r="S3" s="163" t="n"/>
-      <c r="T3" s="163" t="n"/>
-      <c r="U3" s="163" t="n"/>
-      <c r="V3" s="163" t="n"/>
+      <c r="S3" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T3" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U3" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V3" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W3">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X3">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y3">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -31764,10 +31676,34 @@
       <c r="R4" t="n">
         <v>3851.92</v>
       </c>
-      <c r="S4" s="163" t="n"/>
-      <c r="T4" s="163" t="n"/>
-      <c r="U4" s="163" t="n"/>
-      <c r="V4" s="163" t="n"/>
+      <c r="S4" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T4" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U4" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V4" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W4">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X4">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y4">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -31828,10 +31764,34 @@
       <c r="R5" t="n">
         <v>3397.17</v>
       </c>
-      <c r="S5" s="163" t="n"/>
-      <c r="T5" s="163" t="n"/>
-      <c r="U5" s="163" t="n"/>
-      <c r="V5" s="163" t="n"/>
+      <c r="S5" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T5" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U5" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V5" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W5">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X5">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y5">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -31892,10 +31852,34 @@
       <c r="R6" t="n">
         <v>3611.17</v>
       </c>
-      <c r="S6" s="163" t="n"/>
-      <c r="T6" s="163" t="n"/>
-      <c r="U6" s="163" t="n"/>
-      <c r="V6" s="163" t="n"/>
+      <c r="S6" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T6" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U6" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V6" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W6">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X6">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y6">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -31956,10 +31940,34 @@
       <c r="R7" t="n">
         <v>4966.25</v>
       </c>
-      <c r="S7" s="163" t="n"/>
-      <c r="T7" s="163" t="n"/>
-      <c r="U7" s="163" t="n"/>
-      <c r="V7" s="163" t="n"/>
+      <c r="S7" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T7" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U7" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V7" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W7">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X7">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y7">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -32020,10 +32028,34 @@
       <c r="R8" t="n">
         <v>3578.95</v>
       </c>
-      <c r="S8" s="163" t="n"/>
-      <c r="T8" s="163" t="n"/>
-      <c r="U8" s="163" t="n"/>
-      <c r="V8" s="163" t="n"/>
+      <c r="S8" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T8" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U8" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V8" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W8">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X8">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y8">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -32084,10 +32116,34 @@
       <c r="R9" t="n">
         <v>8790</v>
       </c>
-      <c r="S9" s="163" t="n"/>
-      <c r="T9" s="163" t="n"/>
-      <c r="U9" s="163" t="n"/>
-      <c r="V9" s="163" t="n"/>
+      <c r="S9" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T9" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U9" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V9" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W9">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X9">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y9">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -32148,10 +32204,34 @@
       <c r="R10" t="n">
         <v>2000</v>
       </c>
-      <c r="S10" s="163" t="n"/>
-      <c r="T10" s="163" t="n"/>
-      <c r="U10" s="163" t="n"/>
-      <c r="V10" s="163" t="n"/>
+      <c r="S10" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T10" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U10" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V10" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W10">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X10">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y10">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -32212,10 +32292,34 @@
       <c r="R11" t="n">
         <v>4464.26</v>
       </c>
-      <c r="S11" s="163" t="n"/>
-      <c r="T11" s="163" t="n"/>
-      <c r="U11" s="163" t="n"/>
-      <c r="V11" s="163" t="n"/>
+      <c r="S11" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T11" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U11" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V11" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W11">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X11">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y11">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -32276,10 +32380,34 @@
       <c r="R12" t="n">
         <v>4557.73</v>
       </c>
-      <c r="S12" s="163" t="n"/>
-      <c r="T12" s="163" t="n"/>
-      <c r="U12" s="163" t="n"/>
-      <c r="V12" s="163" t="n"/>
+      <c r="S12" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T12" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U12" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V12" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W12">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X12">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y12">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -32340,10 +32468,34 @@
       <c r="R13" t="n">
         <v>20765.73</v>
       </c>
-      <c r="S13" s="163" t="n"/>
-      <c r="T13" s="163" t="n"/>
-      <c r="U13" s="163" t="n"/>
-      <c r="V13" s="163" t="n"/>
+      <c r="S13" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T13" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U13" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V13" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W13">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X13">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y13">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -32404,10 +32556,34 @@
       <c r="R14" t="n">
         <v>5000</v>
       </c>
-      <c r="S14" s="163" t="n"/>
-      <c r="T14" s="163" t="n"/>
-      <c r="U14" s="163" t="n"/>
-      <c r="V14" s="163" t="n"/>
+      <c r="S14" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T14" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U14" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V14" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W14">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X14">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y14">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -32468,10 +32644,34 @@
       <c r="R15" t="n">
         <v>6197.31</v>
       </c>
-      <c r="S15" s="163" t="n"/>
-      <c r="T15" s="163" t="n"/>
-      <c r="U15" s="163" t="n"/>
-      <c r="V15" s="163" t="n"/>
+      <c r="S15" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T15" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U15" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V15" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W15">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X15">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y15">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -32532,10 +32732,34 @@
       <c r="R16" t="n">
         <v>7236.06</v>
       </c>
-      <c r="S16" s="163" t="n"/>
-      <c r="T16" s="163" t="n"/>
-      <c r="U16" s="163" t="n"/>
-      <c r="V16" s="163" t="n"/>
+      <c r="S16" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T16" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U16" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V16" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W16">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X16">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y16">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -32596,10 +32820,34 @@
       <c r="R17" t="n">
         <v>1812.8</v>
       </c>
-      <c r="S17" s="163" t="n"/>
-      <c r="T17" s="163" t="n"/>
-      <c r="U17" s="163" t="n"/>
-      <c r="V17" s="163" t="n"/>
+      <c r="S17" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T17" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U17" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V17" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W17">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X17">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y17">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -32660,10 +32908,34 @@
       <c r="R18" t="n">
         <v>381.27</v>
       </c>
-      <c r="S18" s="163" t="n"/>
-      <c r="T18" s="163" t="n"/>
-      <c r="U18" s="163" t="n"/>
-      <c r="V18" s="163" t="n"/>
+      <c r="S18" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T18" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U18" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V18" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W18">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X18">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y18">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -32724,10 +32996,34 @@
       <c r="R19" t="n">
         <v>31058.46</v>
       </c>
-      <c r="S19" s="163" t="n"/>
-      <c r="T19" s="163" t="n"/>
-      <c r="U19" s="163" t="n"/>
-      <c r="V19" s="163" t="n"/>
+      <c r="S19" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T19" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U19" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V19" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W19">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X19">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y19">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -32788,10 +33084,34 @@
       <c r="R20" t="n">
         <v>5282.81</v>
       </c>
-      <c r="S20" s="163" t="n"/>
-      <c r="T20" s="163" t="n"/>
-      <c r="U20" s="163" t="n"/>
-      <c r="V20" s="163" t="n"/>
+      <c r="S20" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T20" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U20" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V20" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W20">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X20">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y20">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -32852,10 +33172,34 @@
       <c r="R21" t="n">
         <v>34395.51</v>
       </c>
-      <c r="S21" s="163" t="n"/>
-      <c r="T21" s="163" t="n"/>
-      <c r="U21" s="163" t="n"/>
-      <c r="V21" s="163" t="n"/>
+      <c r="S21" s="163">
+        <f>DATE(YEAR(U2),MONTH(U2),1)</f>
+        <v/>
+      </c>
+      <c r="T21" s="163">
+        <f>DATE(YEAR(V2),MONTH(V2),1)</f>
+        <v/>
+      </c>
+      <c r="U21" s="163">
+        <f>D2</f>
+        <v/>
+      </c>
+      <c r="V21" s="163">
+        <f>E2</f>
+        <v/>
+      </c>
+      <c r="W21">
+        <f>U2-V2</f>
+        <v/>
+      </c>
+      <c r="X21">
+        <f>IF(V2&lt;U2,"Antecipação",IF(W2&lt;-5,"Recebimento em Atraso","Recebimento Regular"))</f>
+        <v/>
+      </c>
+      <c r="Y21">
+        <f>IF(X2="Recebimento Regular","Recebimento Regular",IF(ABS(W2)&lt;=15,"Até 15",IF(ABS(W2)&lt;=30,"Entre 15 e 30",IF(ABS(W2)&lt;=60,"Entre 30 e 60",IF(ABS(W2)&lt;=60,"Entre 60 e 90",IF(ABS(W2)&lt;=90,"Entre 90 e 120",IF(ABS(W2)&lt;=120,"Entre 90 e 120",IF(ABS(W2)&lt;=150,"Entre 120 e 150",IF(ABS(W2)&lt;=180,"Entre 150 e 180","Superior a 180")))))))))</f>
+        <v/>
+      </c>
     </row>
     <row r="22"/>
     <row r="23"/>

</xml_diff>